<commit_message>
Where section 5 was a multitester that got rid of the +w (ie shift =0 was best), Section 6 reintroduces this as I haven't been able to confirm this as working on MT4 yet. Also, this section is focussed on backtesting from 1990-2016.
</commit_message>
<xml_diff>
--- a/Ch5 Gasoil4- DD Gasoil Returns Signal Econometric Analysis MultiTester/R0_Trading strategy results_Avg_tester_R4.xlsx
+++ b/Ch5 Gasoil4- DD Gasoil Returns Signal Econometric Analysis MultiTester/R0_Trading strategy results_Avg_tester_R4.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27309"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walsh_pad\Dropbox (Personal)\Further Study\Work\Matlab\phdRepo\matlab\Ch5 Gasoil4- DD Gasoil Returns Signal Econometric Analysis MultiTester\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paddywalsh/Dropbox (Personal)/Further Study/Work/Matlab/phdRepo/matlab/Ch5 Gasoil4- DD Gasoil Returns Signal Econometric Analysis MultiTester/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20700" windowWidth="19180" windowHeight="9470" activeTab="1" xr2:uid="{A23D14C2-9124-4CA5-B2FB-297F6F9491D0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -63,7 +69,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -408,16 +414,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6DDCB8E-239D-46A2-A8AD-F94C58891793}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +452,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -475,7 +481,7 @@
         <v>12.694210070638258</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -504,7 +510,7 @@
         <v>13.446794312960046</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -533,7 +539,7 @@
         <v>13.31542547467876</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -562,7 +568,7 @@
         <v>12.465057602833584</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -591,7 +597,7 @@
         <v>12.164037028280132</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -620,7 +626,7 @@
         <v>10.504014875595198</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -649,7 +655,7 @@
         <v>9.8395501889088575</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -678,7 +684,7 @@
         <v>8.1397822759711289</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -707,7 +713,7 @@
         <v>7.061432958116451</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -736,7 +742,7 @@
         <v>6.735101300318874</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -771,16 +777,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF939716-A2E3-4726-AA3C-1A147CE41C84}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:I13"/>
+      <selection activeCell="A8" sqref="A8:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -809,7 +818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -838,7 +847,7 @@
         <v>13.528340824472695</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -867,7 +876,7 @@
         <v>13.96214524484691</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -896,7 +905,7 @@
         <v>13.847242050298822</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -925,7 +934,7 @@
         <v>12.251535513497517</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -954,7 +963,7 @@
         <v>12.286208382218758</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -983,7 +992,7 @@
         <v>11.806428937576676</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1012,7 +1021,7 @@
         <v>11.50972315221912</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1041,7 +1050,7 @@
         <v>10.457324886040944</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1070,7 +1079,7 @@
         <v>9.9336515055693315</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1099,7 +1108,7 @@
         <v>9.0072513851040501</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>

</xml_diff>